<commit_message>
Update sign up sheet to check the null exception on github actions
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LiveProject_PhpTravels_SignUp_TestData.xlsx
+++ b/src/test/resources/TestData/LiveProject_PhpTravels_SignUp_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{54D6B000-E6C0-482D-A89D-8523A062563A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3B4CA56C-DFE5-4F79-8781-6C471D28D55C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="19545" windowHeight="16500" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="29070" windowHeight="16500" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="testsheet1" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="testsheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G11"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +49,7 @@
     <t>mahmoud.elsharkawy</t>
   </si>
   <si>
-    <t>12345678</t>
+    <t>m1155150745</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -455,7 +455,7 @@
     <col min="2" max="2" width="10.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="1"/>
+    <col min="5" max="5" width="12.75" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished Sign Up on GUI level test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LiveProject_PhpTravels_SignUp_TestData.xlsx
+++ b/src/test/resources/TestData/LiveProject_PhpTravels_SignUp_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3B4CA56C-DFE5-4F79-8781-6C471D28D55C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B46CEE9F-FBDA-4F73-BE95-55511A640C01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="29070" windowHeight="16500" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="29100" windowHeight="16500" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="testsheet1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>FirstName</t>
   </si>
@@ -31,9 +31,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -50,6 +47,30 @@
   </si>
   <si>
     <t>m1155150745</t>
+  </si>
+  <si>
+    <t>TC ID/Name</t>
+  </si>
+  <si>
+    <t>testingValidUserSignUp</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>testingInvalidUserSignUp_emailAlreadyExists</t>
+  </si>
+  <si>
+    <t>testingInvalidUserSignUp_emailWrongFormat</t>
+  </si>
+  <si>
+    <t>Expected Alert Message</t>
+  </si>
+  <si>
+    <t>Email Already Exists.</t>
+  </si>
+  <si>
+    <t>The Email field must contain a valid email address.</t>
   </si>
 </sst>
 </file>
@@ -443,53 +464,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E5A4EB-72C8-0E44-91C4-D3652BB51352}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1155150745</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D3" s="1">
+        <v>1155150745</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
         <v>1155150745</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>